<commit_message>
Data Cleaning in Preprocess, impute missing days -> Regenerate 7 day blocks -> Rerun specific cases
</commit_message>
<xml_diff>
--- a/data/fips-list.xlsx
+++ b/data/fips-list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangz\Dropbox\COVID-tracking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3395F5A2-3CC0-46A5-A5D2-B0784BEC8C97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2000034-184F-4C54-845A-8D60E6428938}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1332" yWindow="60" windowWidth="17280" windowHeight="8964" xr2:uid="{C2FA11B5-500E-496E-9CB7-FEE35B190740}"/>
+    <workbookView xWindow="2892" yWindow="2892" windowWidth="17280" windowHeight="8964" xr2:uid="{C2FA11B5-500E-496E-9CB7-FEE35B190740}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6465" uniqueCount="1992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6467" uniqueCount="1993">
   <si>
     <t>fips</t>
   </si>
@@ -6009,6 +6009,9 @@
   </si>
   <si>
     <t>St. Thomas</t>
+  </si>
+  <si>
+    <t>New York City</t>
   </si>
 </sst>
 </file>
@@ -6360,13 +6363,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723E46BB-4518-44F1-BB3A-5E289442723B}">
-  <dimension ref="A1:C3232"/>
+  <dimension ref="A1:C3233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3232"/>
+    <sheetView tabSelected="1" topLeftCell="A3220" workbookViewId="0">
+      <selection activeCell="F3229" sqref="F3229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -41920,6 +41928,17 @@
         <v>1989</v>
       </c>
     </row>
+    <row r="3233" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3233">
+        <v>99999</v>
+      </c>
+      <c r="B3233" t="s">
+        <v>1992</v>
+      </c>
+      <c r="C3233" t="s">
+        <v>1192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>